<commit_message>
Added Alpha Xi Profiles and Family Trees, Updated Ec and Directors
</commit_message>
<xml_diff>
--- a/src/data/summer21/directors_summer21.xlsx
+++ b/src/data/summer21/directors_summer21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorin\dspuci-website-gatsby\src\data\summer21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\summer21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23AE2BE-1A92-45F6-BEA4-D45BCC6D742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AFCC61-5D72-4E53-8ACF-F0751EDE1883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
+    <workbookView xWindow="4890" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -63,40 +63,31 @@
     <t>Fundraising</t>
   </si>
   <si>
-    <t>Jessie Yang</t>
-  </si>
-  <si>
-    <t>Aarti Vellimedu</t>
-  </si>
-  <si>
-    <t>Marketing Intern</t>
-  </si>
-  <si>
-    <t>Jorina Chen</t>
-  </si>
-  <si>
-    <t>Haley Truong</t>
-  </si>
-  <si>
-    <t>Evelyn Wu</t>
-  </si>
-  <si>
-    <t>Jake Moss</t>
-  </si>
-  <si>
-    <t>Jin Fukusumi</t>
-  </si>
-  <si>
-    <t>Aryan Bajaria</t>
-  </si>
-  <si>
-    <t>Madeline Li</t>
-  </si>
-  <si>
-    <t>Ronica Cheng</t>
-  </si>
-  <si>
     <t>Adora Chen</t>
+  </si>
+  <si>
+    <t>Kevin Cao</t>
+  </si>
+  <si>
+    <t>Jacob Won</t>
+  </si>
+  <si>
+    <t>Mirsab Mirza</t>
+  </si>
+  <si>
+    <t>Kelsie Kim</t>
+  </si>
+  <si>
+    <t>Dylan Tanzil</t>
+  </si>
+  <si>
+    <t>Yoyo Cao</t>
+  </si>
+  <si>
+    <t>David Ayala</t>
+  </si>
+  <si>
+    <t>Safah Faraz</t>
   </si>
 </sst>
 </file>
@@ -462,7 +453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -470,18 +461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2DE730-9C1E-3843-9F88-00F2CA5F5D49}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.69921875" customWidth="1"/>
+    <col min="1" max="1" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -490,104 +481,86 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>